<commit_message>
another semester, another folder
</commit_message>
<xml_diff>
--- a/680 Quantitative Methods/linear_programming/Modeling/Pineapple Production/P1_PineappleLP_bmc.xlsx
+++ b/680 Quantitative Methods/linear_programming/Modeling/Pineapple Production/P1_PineappleLP_bmc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmc/Documents/Projects/OR_KSU/IMSE_680/P1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmccs\OneDrive\Desktop\optimization\680 Quantitative Methods\linear_programming\Modeling\Pineapple Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_BED2BD55B2A5552849FDC6250F788CC4DC4F222C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1CDC71B-735D-4A10-B867-5C7E5F9D9706}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="216" windowWidth="21792" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,16 +90,22 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -242,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,28 +376,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -410,6 +402,21 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -446,7 +453,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -525,7 +538,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -605,7 +624,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -670,7 +695,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -735,7 +766,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1050,32 +1087,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="C16:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="3" customWidth="1"/>
-    <col min="5" max="8" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.83203125" style="3"/>
-    <col min="17" max="17" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.77734375" style="2"/>
+    <col min="3" max="3" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.77734375" style="2"/>
+    <col min="17" max="17" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="16" spans="10:20" ht="19" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:20" ht="18" x14ac:dyDescent="0.3">
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -1089,14 +1128,14 @@
       <c r="N16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
       <c r="J17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,14 +1151,14 @@
       <c r="N17" s="1">
         <v>20000</v>
       </c>
-      <c r="Q17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="3">
+      <c r="Q17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
       <c r="J18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1135,14 +1174,14 @@
       <c r="N18" s="1">
         <v>0</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="Q18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
       <c r="J19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1158,647 +1197,647 @@
       <c r="N19" s="1">
         <v>20000</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="Q19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="Q21" s="2" t="s">
+    <row r="21" spans="3:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="Q21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="Q22" s="3">
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="Q22" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="3:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="5">
         <f>I26-I30</f>
         <v>71300000</v>
       </c>
-      <c r="Q23" s="5" t="s">
+      <c r="Q23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-    </row>
-    <row r="24" spans="3:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q24" s="11" t="s">
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+    </row>
+    <row r="24" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="R24" s="3" t="s">
+      <c r="R24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S24" s="3" t="s">
+      <c r="S24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T24" s="3" t="s">
+      <c r="T24" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="3:20" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="6" t="s">
+    <row r="25" spans="3:20" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25" s="2">
         <v>1.5</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="2">
         <v>0.75</v>
       </c>
-      <c r="S25" s="3">
+      <c r="S25" s="2">
         <v>1.25</v>
       </c>
-      <c r="T25" s="3">
+      <c r="T25" s="2">
         <v>1.25</v>
       </c>
     </row>
-    <row r="26" spans="3:20" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="D26" s="3">
+    <row r="26" spans="3:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="14"/>
+      <c r="D26" s="2">
         <f>Q25*Q28*$Q$22*SUM(K17:K19)</f>
         <v>30000000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f>R25*R28*$Q$22*SUM(L17:L19)</f>
         <v>22500000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <f>S25*S28*$Q$22*SUM(M17:M19)</f>
         <v>12500000</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <f>T25*T28*$Q$22*SUM(N17:N19)</f>
         <v>50000000</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="8">
         <f>SUM(D26:G26)</f>
         <v>115000000</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-    </row>
-    <row r="27" spans="3:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="Q27" s="8" t="s">
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+    </row>
+    <row r="27" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R27" s="8" t="s">
+      <c r="R27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="S27" s="8" t="s">
+      <c r="S27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T27" s="8" t="s">
+      <c r="T27" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="3:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
+    <row r="28" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28" s="2">
         <v>0.5</v>
       </c>
-      <c r="R28" s="3">
+      <c r="R28" s="2">
         <v>1</v>
       </c>
-      <c r="S28" s="3">
+      <c r="S28" s="2">
         <v>1</v>
       </c>
-      <c r="T28" s="3">
+      <c r="T28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:20" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="3">
+    <row r="29" spans="3:20" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="2">
         <f>$Q$35*SUM($K$17:$N$19)</f>
         <v>1200000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <f>R35*SUM($K$17:$N$19)</f>
         <v>24000000</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="3:20" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="6"/>
-      <c r="D30" s="7" t="s">
+    <row r="30" spans="3:20" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="14"/>
+      <c r="D30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="8">
         <f>SUM(E29:F29)+SUM(E31:H31)</f>
         <v>43700000</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="Q30" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-    </row>
-    <row r="31" spans="3:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="3">
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+    </row>
+    <row r="31" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="14"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="2">
         <f>$Q$22*Q32*Q28*SUM(K17:K19)</f>
         <v>4000000</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <f t="shared" ref="F31:H31" si="0">$Q$22*R32*R28*SUM(L17:L19)</f>
         <v>1500000</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <f t="shared" si="0"/>
         <v>3000000</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="Q31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="R31" s="3" t="s">
+      <c r="R31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="S31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="T31" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="Q32" s="3">
+    <row r="32" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="Q32" s="2">
         <v>0.2</v>
       </c>
-      <c r="R32" s="3">
+      <c r="R32" s="2">
         <v>0.05</v>
       </c>
-      <c r="S32" s="3">
+      <c r="S32" s="2">
         <v>0.3</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="Q33" s="2" t="s">
+    <row r="33" spans="3:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="Q33" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-    </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="Q34" s="3" t="s">
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="Q34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R34" s="8" t="s">
+      <c r="R34" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="Q35" s="3">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="Q35" s="2">
         <v>10</v>
       </c>
-      <c r="R35" s="8">
+      <c r="R35" s="4">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C38" s="9" t="s">
+    <row r="38" spans="3:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="C38" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <f>SUM(K17:N17)</f>
         <v>65000</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>40000000</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C40" s="3" t="s">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <f t="shared" ref="D40:D41" si="1">SUM(K18:N18)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>30000000</v>
       </c>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C41" s="3" t="s">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <f t="shared" si="1"/>
         <v>55000</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>50000000</v>
       </c>
     </row>
-    <row r="42" spans="3:20" ht="19" x14ac:dyDescent="0.2">
-      <c r="C42" s="9" t="s">
+    <row r="42" spans="3:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="C42" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C43" s="14" t="s">
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C43" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <f>Q28*Q22*SUM(K17:K19)</f>
         <v>20000000</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>20000000</v>
       </c>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C44" s="14" t="s">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C44" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <f>Q22*SUM(L17:L19)</f>
         <v>30000000</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>30000000</v>
       </c>
     </row>
-    <row r="45" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="15" t="s">
+    <row r="45" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <f>(Q22*SUM(M17:M19))+(Q22*SUM(N17:N19))</f>
         <v>50000000</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>50000000</v>
       </c>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C46" s="14" t="s">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C46" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <f>Q28*Q22*SUM(K17:K19)</f>
         <v>20000000</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46" s="3">
+      <c r="E46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="2">
         <v>10000000</v>
       </c>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C47" s="14" t="s">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C47" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <f>Q22*SUM(L17:L19)</f>
         <v>30000000</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F47" s="3">
+      <c r="E47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="2">
         <v>10000000</v>
       </c>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C48" s="14" t="s">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C48" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <f>Q22*SUM(M17:M19)</f>
         <v>10000000</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="3">
+      <c r="E48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="2">
         <v>10000000</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C49" s="14" t="s">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <f>Q22*SUM(N17:N19)</f>
         <v>40000000</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F49" s="3">
+      <c r="E49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F49" s="2">
         <v>10000000</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C50" s="14" t="s">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <f>(K17*R17+K18*R18+K19*R19) -7.5*SUM(K17:K19)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C51" s="14" t="s">
+      <c r="E50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <f>(L17*R17+L18*R18+L19*R19)-9*SUM(L17:L19)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C52" s="14" t="s">
+      <c r="E51" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <f>(M17*R17+M18*R18+M19*R19)-8*SUM(M17:M19)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C53" s="14" t="s">
+      <c r="E52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <f>(N17*R17+N18*R18+N19*R19)-8*SUM(N17:N19)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="C54" s="9" t="s">
+      <c r="E53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="C54" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C55" s="14">
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="9">
         <f>K17</f>
         <v>10000</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C56" s="14">
+      <c r="D55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="9">
         <f t="shared" ref="C56:C57" si="2">K18</f>
         <v>0</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C57" s="14">
+      <c r="D56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="9">
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C58" s="3">
+      <c r="D57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="2">
         <f>L17</f>
         <v>30000</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E58" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C59" s="3">
+      <c r="D58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="2">
         <f t="shared" ref="C59:C60" si="3">L18</f>
         <v>0</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C60" s="3">
+      <c r="D59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C61" s="3">
+      <c r="D60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="2">
         <f>M17</f>
         <v>5000</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C62" s="3">
+      <c r="D61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="2">
         <f t="shared" ref="C62:C63" si="4">M18</f>
         <v>0</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C63" s="3">
+      <c r="D62" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="2">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C64" s="3">
+      <c r="D63" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="2">
         <f>N17</f>
         <v>20000</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C65" s="3">
+      <c r="D64" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C65" s="2">
         <f t="shared" ref="C65:C66" si="5">N18</f>
         <v>0</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C66" s="3">
+      <c r="D65" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="2">
         <f t="shared" si="5"/>
         <v>20000</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="3">
+      <c r="D66" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>